<commit_message>
Adding new United States geography keyword
</commit_message>
<xml_diff>
--- a/archive/Keywords.xlsx
+++ b/archive/Keywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/bibliophilly-keywords-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/bibliophilly-keywords-/archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4A0CB3-E605-F945-9F1B-FE923A69A167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4821A243-B5CF-9940-8326-320040C83C83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="287">
   <si>
     <t>Book Type</t>
   </si>
@@ -878,6 +878,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -894,15 +897,18 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1264,8 +1270,8 @@
   </sheetPr>
   <dimension ref="A1:BL1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1946,10 +1952,13 @@
       <c r="AK5" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AL5" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="AM5" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AM5" s="2" t="s">
+      <c r="AN5" s="2" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>